<commit_message>
volumes and pages done, now redoing interactions
</commit_message>
<xml_diff>
--- a/data/Ralph_Azham/_all.xlsx
+++ b/data/Ralph_Azham/_all.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\Eclipse\workspaces\Networks\NaNet\data\Ralph_Azham\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Vincent\eclipse\workspaces\Networks\NaNet\data\Ralph_Azham\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Interactions" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Interactions!$A$1:$X$981</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3772" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3784" uniqueCount="497">
   <si>
     <t>Page</t>
   </si>
@@ -1509,11 +1509,47 @@
   <si>
     <t>StartPanel</t>
   </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Est-ce qu'on ment aux gens qu'on aime ?</t>
+  </si>
+  <si>
+    <t>La mort au début du chemin</t>
+  </si>
+  <si>
+    <t>Noires sont les étoiles</t>
+  </si>
+  <si>
+    <t>Un caillou enterré n'apprend jamais rien</t>
+  </si>
+  <si>
+    <t>L'ennemi de mon ennemi</t>
+  </si>
+  <si>
+    <t>Une fin à toute chose</t>
+  </si>
+  <si>
+    <t>Personne n'attrape une rivière</t>
+  </si>
+  <si>
+    <t>Point de rupture</t>
+  </si>
+  <si>
+    <t>Un feu qui meurt</t>
+  </si>
+  <si>
+    <t>L'engrenage</t>
+  </si>
+  <si>
+    <t>Le pays des démons bleus</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1582,7 +1618,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1597,6 +1633,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1879,9 +1918,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X982"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37478,10 +37517,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37490,9 +37529,10 @@
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -37505,8 +37545,11 @@
       <c r="D1" s="2" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="12" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -37520,8 +37563,11 @@
         <f t="shared" ref="D2:D12" si="0">C2-B2+1</f>
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -37536,8 +37582,11 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -37552,8 +37601,11 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -37568,8 +37620,11 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="3" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -37584,8 +37639,11 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -37600,8 +37658,11 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -37616,8 +37677,11 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -37632,8 +37696,11 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="3" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -37648,8 +37715,11 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -37664,8 +37734,11 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -37680,8 +37753,11 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
finished updating code for more generic file format, must still debug
</commit_message>
<xml_diff>
--- a/data/Ralph_Azham/_all.xlsx
+++ b/data/Ralph_Azham/_all.xlsx
@@ -1919,8 +1919,8 @@
   <dimension ref="A1:X982"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A905" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E936" sqref="E936"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6193,7 +6193,7 @@
         <v>7</v>
       </c>
       <c r="D151" s="4">
-        <v>196</v>
+        <v>106</v>
       </c>
       <c r="E151" s="4">
         <v>9</v>
@@ -8577,7 +8577,7 @@
         <v>161</v>
       </c>
       <c r="E239" s="4">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F239" s="4" t="s">
         <v>20</v>
@@ -8647,7 +8647,7 @@
         <v>162</v>
       </c>
       <c r="E241" s="4">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F241" s="4" t="s">
         <v>20</v>
@@ -12241,7 +12241,7 @@
         <v>13</v>
       </c>
       <c r="D364" s="4">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E364" s="4">
         <v>9</v>
@@ -12851,7 +12851,7 @@
         <v>1</v>
       </c>
       <c r="D387" s="4">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E387" s="4">
         <v>13</v>
@@ -13447,7 +13447,7 @@
         <v>4</v>
       </c>
       <c r="D409" s="4">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E409" s="4">
         <v>8</v>
@@ -19612,6 +19612,9 @@
       <c r="D616">
         <v>330</v>
       </c>
+      <c r="E616">
+        <v>7</v>
+      </c>
       <c r="F616" s="4" t="s">
         <v>15</v>
       </c>
@@ -20951,7 +20954,7 @@
         <v>358</v>
       </c>
       <c r="E667" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F667" t="s">
         <v>20</v>
@@ -25476,7 +25479,7 @@
         <v>435</v>
       </c>
       <c r="E825" s="4">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F825" t="s">
         <v>20</v>
@@ -25637,7 +25640,7 @@
         <v>439</v>
       </c>
       <c r="E829" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F829" t="s">
         <v>20</v>
@@ -28638,7 +28641,7 @@
         <v>496</v>
       </c>
       <c r="E935" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F935" s="4" t="s">
         <v>37</v>
@@ -29916,8 +29919,8 @@
   <dimension ref="A1:C898"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A477" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B497" sqref="B497"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
improved plotting, corrected few minor bugs
</commit_message>
<xml_diff>
--- a/data/Ralph_Azham/_all.xlsx
+++ b/data/Ralph_Azham/_all.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Vincent\eclipse\workspaces\Networks\NaNet\data\Ralph_Azham\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\Eclipse\workspaces\Networks\NaNet\data\Ralph_Azham\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Interactions" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Interactions!$A$1:$X$981</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5104" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5103" uniqueCount="540">
   <si>
     <t>Page</t>
   </si>
@@ -1679,7 +1679,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2058,9 +2058,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X982"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A943" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A982" sqref="A982"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A904" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A913" sqref="A913"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28145,7 +28145,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="913" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="913" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A913" s="4">
         <v>11</v>
       </c>
@@ -28213,13 +28213,10 @@
         <v>356</v>
       </c>
       <c r="W913" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="X913" s="4" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="914" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="914" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A914" s="4">
         <v>11</v>
       </c>
@@ -28248,7 +28245,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="915" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="915" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A915" s="4">
         <v>11</v>
       </c>
@@ -28271,7 +28268,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="916" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="916" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A916" s="4">
         <v>11</v>
       </c>
@@ -28300,7 +28297,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="917" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="917" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A917" s="4">
         <v>11</v>
       </c>
@@ -28326,7 +28323,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="918" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="918" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A918" s="4">
         <v>11</v>
       </c>
@@ -28349,7 +28346,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="919" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="919" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A919" s="4">
         <v>11</v>
       </c>
@@ -28375,7 +28372,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="920" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="920" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A920" s="4">
         <v>11</v>
       </c>
@@ -28404,7 +28401,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="921" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="921" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A921" s="4">
         <v>11</v>
       </c>
@@ -28433,7 +28430,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="922" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="922" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A922" s="4">
         <v>11</v>
       </c>
@@ -28465,7 +28462,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="923" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="923" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A923" s="4">
         <v>11</v>
       </c>
@@ -28497,7 +28494,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="924" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="924" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A924" s="4">
         <v>11</v>
       </c>
@@ -28525,7 +28522,7 @@
       <c r="I924" s="4"/>
       <c r="J924" s="4"/>
     </row>
-    <row r="925" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="925" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A925" s="4">
         <v>11</v>
       </c>
@@ -28548,7 +28545,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="926" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="926" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A926" s="4">
         <v>11</v>
       </c>
@@ -28571,7 +28568,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="927" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="927" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A927" s="4">
         <v>11</v>
       </c>
@@ -28597,7 +28594,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="928" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="928" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A928" s="4">
         <v>11</v>
       </c>
@@ -37924,7 +37921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C439"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B401" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>